<commit_message>
update institutions and contributorType.xlsx
</commit_message>
<xml_diff>
--- a/data/excel/contributorType.xlsx
+++ b/data/excel/contributorType.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moon.ntkcz.cz\petka\NUŠL\SW\INVENIO 3\taxonomie\taxonomies_od_Dana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moon.ntkcz.cz\petka\NUŠL\SW\INVENIO 3\taxonomie\současné_hotové\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5890" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5892" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="127">
   <si>
     <t>code</t>
   </si>
@@ -348,6 +348,63 @@
   </si>
   <si>
     <t>pan</t>
+  </si>
+  <si>
+    <t>data-collector</t>
+  </si>
+  <si>
+    <t>data collector</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>pbl</t>
+  </si>
+  <si>
+    <t>proofreader</t>
+  </si>
+  <si>
+    <t>pfr</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>own</t>
+  </si>
+  <si>
+    <t>former-owner</t>
+  </si>
+  <si>
+    <t>fmo</t>
+  </si>
+  <si>
+    <t>respondent</t>
+  </si>
+  <si>
+    <t>rsp</t>
+  </si>
+  <si>
+    <t>DataCollector</t>
+  </si>
+  <si>
+    <t>nakladatel</t>
+  </si>
+  <si>
+    <t>majitel</t>
+  </si>
+  <si>
+    <t>dřívější majitel</t>
+  </si>
+  <si>
+    <t>former owner</t>
+  </si>
+  <si>
+    <t>korektor</t>
+  </si>
+  <si>
+    <t>sběratel dat</t>
   </si>
 </sst>
 </file>
@@ -389,7 +446,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -406,11 +463,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -424,8 +490,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -712,20 +786,20 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.90625" style="1" customWidth="1"/>
-    <col min="9" max="1024" width="11.54296875" style="1"/>
+    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
+    <col min="9" max="1024" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -741,7 +815,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -757,7 +831,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -780,7 +854,7 @@
       <c r="H5"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -799,597 +873,686 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>47</v>
+      <c r="B15" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G33"/>
       <c r="H33"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
+        <v>1</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
+        <v>1</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
+        <v>1</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="11">
+        <v>1</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E44" s="5"/>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="E50" s="8"/>
-    </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="E55" s="8"/>
-    </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="7"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="7"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D60" s="5"/>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-    </row>
-    <row r="93" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="93" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>